<commit_message>
telex BOM update; command-reference update
</commit_message>
<xml_diff>
--- a/hardware/TELEXo/board/TELEXo-BOM.xlsx
+++ b/hardware/TELEXo/board/TELEXo-BOM.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="Telex_O" localSheetId="0">TELEXo!#REF!</definedName>
-    <definedName name="Telex_O_1" localSheetId="0">TELEXo!$A$1:$J$29</definedName>
+    <definedName name="Telex_O_1" localSheetId="0">TELEXo!$A$1:$J$28</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="122">
   <si>
     <t>LM4040A10IDBZR</t>
   </si>
@@ -436,9 +436,6 @@
   </si>
   <si>
     <t>R102,R103,R104,R105</t>
-  </si>
-  <si>
-    <t>279-CPF0603F10KC1</t>
   </si>
   <si>
     <t>R1,R2,R3,R4,R5,R6,R7,R8</t>
@@ -700,8 +697,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:J29" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:J28" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J28"/>
   <sortState ref="A2:J28">
     <sortCondition ref="E1:E28"/>
   </sortState>
@@ -984,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,7 +1308,7 @@
         <v>50</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2">
         <v>1206</v>
@@ -1529,7 +1526,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>86</v>
@@ -1543,96 +1540,76 @@
       <c r="E25" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="F25" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="G25" s="1" t="s">
         <v>119</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>1</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E29" s="2" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mid-process update for TXi
</commit_message>
<xml_diff>
--- a/hardware/TELEXo/board/TELEXo-BOM.xlsx
+++ b/hardware/TELEXo/board/TELEXo-BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24680" yWindow="7980" windowWidth="25920" windowHeight="17900" tabRatio="500"/>
+    <workbookView xWindow="17100" yWindow="6340" windowWidth="25920" windowHeight="17900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TELEXo" sheetId="1" r:id="rId1"/>
@@ -983,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>83</v>
@@ -1517,6 +1517,9 @@
       <c r="E24" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="G24" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="I24" s="1" t="s">
         <v>117</v>
       </c>
@@ -1526,7 +1529,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>85</v>
@@ -1542,9 +1545,6 @@
       </c>
       <c r="F25" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
updated build map and BOM for 1k trigger out resistor reversion; massively improved the smoothing method for the TXi reads; added back the Teensy-specific i2c library for the TXo (oops)
</commit_message>
<xml_diff>
--- a/hardware/TELEXo/board/TELEXo-BOM.xlsx
+++ b/hardware/TELEXo/board/TELEXo-BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24680" yWindow="7980" windowWidth="25920" windowHeight="17900" tabRatio="500"/>
+    <workbookView xWindow="19660" yWindow="7980" windowWidth="30940" windowHeight="17900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TELEXo" sheetId="1" r:id="rId1"/>
@@ -984,7 +984,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>83</v>
@@ -1517,6 +1517,9 @@
       <c r="E24" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="G24" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="I24" s="1" t="s">
         <v>117</v>
       </c>
@@ -1526,7 +1529,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>85</v>
@@ -1542,9 +1545,6 @@
       </c>
       <c r="F25" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
bom fix; txo envelope recomputation enhancement; telexi smoothing enhancement
</commit_message>
<xml_diff>
--- a/hardware/TELEXo/board/TELEXo-BOM.xlsx
+++ b/hardware/TELEXo/board/TELEXo-BOM.xlsx
@@ -507,7 +507,7 @@
     <t>Capacitor; &gt;=16V; 1%</t>
   </si>
   <si>
-    <t>Substitue 110p if you plan to use a Teensy 3.6; Mouser PN 81-GRM185C1H111FA01D</t>
+    <t>Substitue 110p if you plan to use a Teensy 3.6; Mouser PN 80-C1206C111J1G</t>
   </si>
 </sst>
 </file>
@@ -587,20 +587,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Avenir Next Regular"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -811,6 +797,20 @@
         <name val="Avenir Next Regular"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Avenir Next Regular"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -830,24 +830,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:L31" totalsRowShown="0" headerRowDxfId="13" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:L31" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:L31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A2:L31">
     <sortCondition ref="C1:C31"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Qty" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Device" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Package" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Description" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="TopTop" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TopBottom" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="BottomBottom" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BottomTop" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="OC_MOUSER" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{AEDD9F90-6F54-1840-A8F3-7FDE3ED9AB42}" name="URL" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{E427EAEB-0E87-A446-8D9D-EAA405B01937}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Qty" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Device" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Package" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Description" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="TopTop" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TopBottom" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="BottomBottom" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BottomTop" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="OC_MOUSER" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{AEDD9F90-6F54-1840-A8F3-7FDE3ED9AB42}" name="URL" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{E427EAEB-0E87-A446-8D9D-EAA405B01937}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1118,7 +1118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -1582,7 +1582,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" s="4" customFormat="1" ht="30">
+    <row r="19" spans="1:12" s="4" customFormat="1" ht="45">
       <c r="A19" s="4">
         <v>8</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="4" customFormat="1" ht="30">
+    <row r="20" spans="1:12" s="4" customFormat="1" ht="45">
       <c r="A20" s="4">
         <v>4</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="4" customFormat="1" ht="30">
+    <row r="21" spans="1:12" s="4" customFormat="1" ht="45">
       <c r="A21" s="4">
         <v>4</v>
       </c>

</xml_diff>